<commit_message>
add entity resolution part improve selection strategies
</commit_message>
<xml_diff>
--- a/referenceMappingStats/ontology_coverage.xlsx
+++ b/referenceMappingStats/ontology_coverage.xlsx
@@ -14,10 +14,11 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId2"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId3"/>
+    <sheet name="coverage_comb" sheetId="2" r:id="rId3"/>
+    <sheet name="relations" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="referenceConceptStat" localSheetId="2">Tabelle2!$A$1:$B$85</definedName>
+    <definedName name="referenceConceptStat" localSheetId="2">coverage_comb!$A$6:$B$90</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="138">
   <si>
     <t>LNC</t>
   </si>
@@ -296,24 +297,12 @@
     <t>NEU</t>
   </si>
   <si>
-    <t>Concepts Reference mapping</t>
-  </si>
-  <si>
-    <t>SAB</t>
-  </si>
-  <si>
-    <t>Count(Distinct(umls.CUI))</t>
-  </si>
-  <si>
     <t>Combination</t>
   </si>
   <si>
     <t>#concepts</t>
   </si>
   <si>
-    <t>sizeOrder</t>
-  </si>
-  <si>
     <t>MDR,CHV</t>
   </si>
   <si>
@@ -354,13 +343,127 @@
   </si>
   <si>
     <t>#forms</t>
+  </si>
+  <si>
+    <t>Coverage of each ontology according to the reference mapping</t>
+  </si>
+  <si>
+    <t>Size of ontologies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concepts Reference mapping: </t>
+  </si>
+  <si>
+    <t>ontology</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>total missing annotations</t>
+  </si>
+  <si>
+    <t>UMLS Relations</t>
+  </si>
+  <si>
+    <t>PAR</t>
+  </si>
+  <si>
+    <t>different ontology combination and ist coverage ratio</t>
+  </si>
+  <si>
+    <t>CUI1</t>
+  </si>
+  <si>
+    <t>Schema</t>
+  </si>
+  <si>
+    <t>REL</t>
+  </si>
+  <si>
+    <t>RELA</t>
+  </si>
+  <si>
+    <t>CUI2</t>
+  </si>
+  <si>
+    <t>C[0-9]{7}</t>
+  </si>
+  <si>
+    <t>PAR'|'CHD'|null</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>CUI1--&gt;CUI2</t>
+  </si>
+  <si>
+    <t>Interpretation</t>
+  </si>
+  <si>
+    <t>graph</t>
+  </si>
+  <si>
+    <t>CHD</t>
+  </si>
+  <si>
+    <t>CUI1&lt;--CUI2</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>Cui2 is parent of CUI1</t>
+  </si>
+  <si>
+    <t>Cui2 is child of CUI1</t>
+  </si>
+  <si>
+    <t>C0729760-inverse_isa-&gt;C0000102 ( Chemical categorised functionally)-inverse_isa-&gt; (1-naphthylamine)</t>
+  </si>
+  <si>
+    <t>has_branch</t>
+  </si>
+  <si>
+    <t>has_member</t>
+  </si>
+  <si>
+    <t>has_part</t>
+  </si>
+  <si>
+    <t>has_tributary</t>
+  </si>
+  <si>
+    <t>inverse_isa</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>branch_of</t>
+  </si>
+  <si>
+    <t>isa</t>
+  </si>
+  <si>
+    <t>member_of</t>
+  </si>
+  <si>
+    <t>part_of</t>
+  </si>
+  <si>
+    <t>tributary_of</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,8 +471,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -394,6 +520,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -407,7 +539,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -417,6 +549,32 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -703,7 +861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B84"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B19"/>
     </sheetView>
   </sheetViews>
@@ -1408,1008 +1566,1002 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L85"/>
+  <dimension ref="A2:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1"/>
-    <col min="8" max="8" width="33.28515625" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
+    <col min="10" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="14">
+        <v>4902</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="20"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="H5" s="21"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D6" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>3429</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="13">
+        <v>906637</v>
+      </c>
+      <c r="G7" t="s">
         <v>86</v>
       </c>
-      <c r="C1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="3">
-        <v>906637</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="H7">
+        <v>3489</v>
+      </c>
+      <c r="I7" s="8">
+        <f t="shared" ref="I7:I15" si="0">H7/$C$2</f>
+        <v>0.71175030599755207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>3237</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="9">
+        <v>347770</v>
+      </c>
+      <c r="G8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8">
+        <v>4182</v>
+      </c>
+      <c r="I8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.85312117503059981</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9">
+        <v>2993</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B2">
-        <v>3429</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="7">
+      <c r="E9" s="9">
         <v>334921</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="5">
-        <v>347770</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>3237</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1">
-        <v>56380</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="7">
-        <v>334921</v>
-      </c>
-      <c r="H3" t="s">
-        <v>87</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="G9" t="s">
         <v>88</v>
       </c>
-      <c r="J3" t="s">
-        <v>100</v>
-      </c>
-      <c r="K3" t="s">
-        <v>99</v>
-      </c>
-      <c r="L3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4">
-        <v>2993</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>110035</v>
-      </c>
-      <c r="E4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="1">
-        <v>314206</v>
-      </c>
-      <c r="H4" t="s">
-        <v>90</v>
-      </c>
-      <c r="I4">
-        <v>3489</v>
-      </c>
-      <c r="J4" s="8">
-        <f>I4/$H$22</f>
-        <v>0.71175030599755207</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>2906</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1">
-        <v>170199</v>
-      </c>
-      <c r="E5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" s="1">
-        <v>258491</v>
-      </c>
-      <c r="H5" t="s">
-        <v>91</v>
-      </c>
-      <c r="I5">
-        <v>4182</v>
-      </c>
-      <c r="J5" s="8">
-        <f t="shared" ref="J5:J12" si="0">I5/$H$22</f>
-        <v>0.85312117503059981</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6">
-        <v>2150</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5">
-        <v>347770</v>
-      </c>
-      <c r="E6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="1">
-        <v>178191</v>
-      </c>
-      <c r="H6" t="s">
-        <v>92</v>
-      </c>
-      <c r="I6">
+      <c r="H9">
         <v>4384</v>
       </c>
-      <c r="J6" s="8">
+      <c r="I9" s="8">
         <f t="shared" si="0"/>
         <v>0.89432884536923707</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7">
-        <v>1502</v>
-      </c>
-      <c r="C7">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1">
-        <v>50039</v>
-      </c>
-      <c r="E7" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="1">
-        <v>170199</v>
-      </c>
-      <c r="H7" t="s">
-        <v>93</v>
-      </c>
-      <c r="I7">
+      <c r="B10">
+        <v>2906</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="1">
+        <v>314206</v>
+      </c>
+      <c r="G10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10">
         <v>4681</v>
       </c>
-      <c r="J7" s="8">
+      <c r="I10" s="8">
         <f t="shared" si="0"/>
         <v>0.95491636066911467</v>
       </c>
-      <c r="K7">
+      <c r="J10">
         <v>555961</v>
       </c>
-      <c r="L7">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8">
-        <v>1456</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1">
-        <v>314206</v>
-      </c>
-      <c r="E8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>146712</v>
-      </c>
-      <c r="H8" t="s">
-        <v>94</v>
-      </c>
-      <c r="I8">
+      <c r="K10">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11">
+        <v>2150</v>
+      </c>
+      <c r="D11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="1">
+        <v>258491</v>
+      </c>
+      <c r="G11" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11">
         <v>4457</v>
       </c>
-      <c r="J8" s="8">
+      <c r="I11" s="8">
         <f t="shared" si="0"/>
         <v>0.90922072623419015</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9">
-        <v>1379</v>
-      </c>
-      <c r="E9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="1">
-        <v>110035</v>
-      </c>
-      <c r="H9" t="s">
-        <v>95</v>
-      </c>
-      <c r="I9">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>1502</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="1">
+        <v>178191</v>
+      </c>
+      <c r="G12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12">
         <v>4384</v>
       </c>
-      <c r="J9" s="8">
+      <c r="I12" s="8">
         <f t="shared" si="0"/>
         <v>0.89432884536923707</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>1298</v>
-      </c>
-      <c r="E10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="1">
-        <v>98902</v>
-      </c>
-      <c r="H10" t="s">
-        <v>96</v>
-      </c>
-      <c r="I10">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13">
+        <v>1456</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>170199</v>
+      </c>
+      <c r="G13" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13">
         <v>4576</v>
       </c>
-      <c r="J10" s="8">
+      <c r="I13" s="8">
         <f t="shared" si="0"/>
         <v>0.93349653202774374</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B11">
-        <v>1188</v>
-      </c>
-      <c r="E11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="1">
-        <v>82042</v>
-      </c>
-      <c r="H11" t="s">
-        <v>97</v>
-      </c>
-      <c r="I11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14">
+        <v>1379</v>
+      </c>
+      <c r="D14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>146712</v>
+      </c>
+      <c r="G14" t="s">
+        <v>93</v>
+      </c>
+      <c r="H14">
         <v>3823</v>
       </c>
-      <c r="J11" s="8">
+      <c r="I14" s="8">
         <f t="shared" si="0"/>
         <v>0.77988576091391271</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12">
-        <v>1067</v>
-      </c>
-      <c r="E12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="1">
-        <v>81492</v>
-      </c>
-      <c r="H12" t="s">
-        <v>98</v>
-      </c>
-      <c r="I12">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>1298</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="1">
+        <v>110035</v>
+      </c>
+      <c r="G15" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15">
         <v>4745</v>
       </c>
-      <c r="J12" s="8">
+      <c r="I15" s="8">
         <f t="shared" si="0"/>
         <v>0.96797225622195027</v>
       </c>
-      <c r="K12">
+      <c r="J15">
         <v>850069</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13">
-        <v>1009</v>
-      </c>
-      <c r="E13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="1">
-        <v>61179</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14">
-        <v>737</v>
-      </c>
-      <c r="E14" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="1">
-        <v>60211</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>628</v>
-      </c>
-      <c r="E15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="1">
-        <v>57227</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="B16">
-        <v>605</v>
-      </c>
-      <c r="E16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="1">
-        <v>56380</v>
+        <v>1188</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="1">
+        <v>98902</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>600</v>
-      </c>
-      <c r="E17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="1">
-        <v>50039</v>
+        <v>1067</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="1">
+        <v>82042</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="B18">
-        <v>586</v>
-      </c>
-      <c r="E18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="1">
-        <v>39619</v>
+        <v>1009</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="1">
+        <v>81492</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B19">
-        <v>584</v>
-      </c>
-      <c r="E19" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="1">
-        <v>38703</v>
+        <v>737</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="1">
+        <v>61179</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="B20">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>628</v>
+      </c>
+      <c r="D20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="1">
+        <v>60211</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B21">
-        <v>482</v>
+        <v>605</v>
+      </c>
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="1">
+        <v>57227</v>
+      </c>
+      <c r="G21" t="s">
+        <v>99</v>
       </c>
       <c r="H21" t="s">
-        <v>84</v>
-      </c>
-      <c r="I21" t="s">
-        <v>100</v>
+        <v>98</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B22">
-        <v>473</v>
+        <v>600</v>
       </c>
       <c r="D22" t="s">
-        <v>103</v>
-      </c>
-      <c r="E22" t="s">
-        <v>102</v>
-      </c>
-      <c r="F22" t="s">
-        <v>101</v>
+        <v>11</v>
+      </c>
+      <c r="E22" s="1">
+        <v>56380</v>
+      </c>
+      <c r="G22">
+        <v>25</v>
       </c>
       <c r="H22">
-        <v>4902</v>
+        <v>544</v>
+      </c>
+      <c r="I22">
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B23">
-        <v>457</v>
-      </c>
-      <c r="D23">
-        <v>25</v>
-      </c>
-      <c r="E23">
-        <v>544</v>
-      </c>
-      <c r="F23">
-        <v>3</v>
+        <v>586</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="1">
+        <v>50039</v>
+      </c>
+      <c r="G23">
+        <v>421</v>
+      </c>
+      <c r="H23">
+        <v>25710</v>
+      </c>
+      <c r="I23">
+        <v>464</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B24">
-        <v>451</v>
+        <v>584</v>
+      </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="1">
+        <v>39619</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B25">
-        <v>429</v>
+        <v>508</v>
+      </c>
+      <c r="D25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="1">
+        <v>38703</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B26">
-        <v>417</v>
+        <v>482</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B27">
-        <v>389</v>
+        <v>473</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="B28">
-        <v>379</v>
+        <v>457</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B29">
-        <v>373</v>
+        <v>451</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="B30">
-        <v>370</v>
+        <v>429</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="B31">
-        <v>346</v>
+        <v>417</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="B32">
-        <v>317</v>
+        <v>389</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="B33">
-        <v>290</v>
+        <v>379</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B34">
-        <v>269</v>
+        <v>373</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B35">
-        <v>190</v>
+        <v>370</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B36">
-        <v>174</v>
+        <v>346</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B37">
-        <v>172</v>
+        <v>317</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B38">
-        <v>171</v>
+        <v>290</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="B39">
-        <v>157</v>
+        <v>269</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="B40">
-        <v>152</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B41">
-        <v>137</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B42">
-        <v>113</v>
+        <v>172</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="B43">
-        <v>113</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="B44">
-        <v>111</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B45">
-        <v>104</v>
+        <v>152</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B46">
-        <v>94</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B47">
-        <v>88</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B48">
-        <v>67</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B49">
-        <v>54</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B50">
-        <v>54</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="B51">
-        <v>51</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="B52">
-        <v>48</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="B53">
-        <v>47</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B54">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B55">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="B56">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="B57">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="B58">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B59">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B60">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="B61">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="B62">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B63">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B64">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B65">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B66">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="B67">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="B68">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B69">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B70">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B71">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="B72">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B73">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="B74">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B75">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="B76">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B77">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B78">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="B79">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="B80">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B81">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B82">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="B83">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>13</v>
       </c>
       <c r="B84">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>56</v>
+      </c>
+      <c r="B85">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>33</v>
+      </c>
+      <c r="B86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>44</v>
+      </c>
+      <c r="B87">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>70</v>
+      </c>
+      <c r="B88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>83</v>
+      </c>
+      <c r="B89">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>43</v>
       </c>
-      <c r="B85">
+      <c r="B90">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B85">
+  <sortState ref="A7:B90">
     <sortCondition descending="1" ref="B2:B85"/>
   </sortState>
-  <conditionalFormatting sqref="I4:I11">
+  <mergeCells count="4">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H7:H14">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2421,7 +2573,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
+  <conditionalFormatting sqref="H15">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2434,5 +2586,205 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10">
+        <v>2313575</v>
+      </c>
+      <c r="E10" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10">
+        <v>2313575</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11">
+        <v>5327</v>
+      </c>
+      <c r="E11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11">
+        <v>5327</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12">
+        <v>8116</v>
+      </c>
+      <c r="E12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F12">
+        <v>2251675</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13">
+        <v>19436</v>
+      </c>
+      <c r="E13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13">
+        <v>8116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14">
+        <v>1659</v>
+      </c>
+      <c r="E14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F14">
+        <v>19436</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15">
+        <v>2251675</v>
+      </c>
+      <c r="E15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F15">
+        <v>1659</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>